<commit_message>
chore: Remove splitRatios sheet
</commit_message>
<xml_diff>
--- a/io/input/tutorial_02_adenine_cycle.xlsx
+++ b/io/input/tutorial_02_adenine_cycle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,14 +13,13 @@
     <sheet name="rxns" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="mets" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="poolConst" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="splitRatios" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="thermo_ineq_constraints" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="thermoRxns" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="thermoMets" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="measRates" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="protData" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="metsData" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="kinetics1" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="thermo_ineq_constraints" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="thermoRxns" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="thermoMets" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="measRates" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="protData" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="metsData" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="kinetics1" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -191,9 +190,6 @@
   </si>
   <si>
     <t xml:space="preserve">rhs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref</t>
   </si>
   <si>
     <t xml:space="preserve">∆Gr'_min (kJ/mol)</t>
@@ -446,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -559,10 +555,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -582,7 +574,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -590,7 +582,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,198 +1735,231 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="16.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="25" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="25" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="25" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.6"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="19" t="s">
+      <c r="M1" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="P1" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="21" t="n">
-        <v>1.121</v>
-      </c>
-      <c r="C2" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="23" t="n">
-        <v>0.1601</v>
-      </c>
-      <c r="E2" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="23" t="n">
-        <v>0.4209</v>
-      </c>
-      <c r="G2" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="23" t="n">
-        <v>0.6359</v>
-      </c>
-      <c r="I2" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="24" t="n">
-        <v>2.5904</v>
-      </c>
-      <c r="K2" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="24" t="n">
-        <v>2.9387</v>
-      </c>
-      <c r="M2" s="22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="E2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="H2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="K2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="N2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="21" t="n">
-        <v>1.121</v>
-      </c>
-      <c r="C3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="23" t="n">
-        <v>0.1601</v>
-      </c>
-      <c r="E3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="23" t="n">
-        <v>0.4209</v>
-      </c>
-      <c r="G3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="23" t="n">
-        <v>0.6359</v>
-      </c>
-      <c r="I3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="24" t="n">
-        <v>2.5904</v>
-      </c>
-      <c r="K3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="24" t="n">
-        <v>2.9387</v>
-      </c>
-      <c r="M3" s="22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="E3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="H3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="K3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="N3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="21" t="n">
-        <f aca="false">2*B3</f>
-        <v>2.242</v>
-      </c>
-      <c r="C4" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="23" t="n">
-        <f aca="false">2*D3</f>
-        <v>0.3202</v>
-      </c>
-      <c r="E4" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="23" t="n">
-        <f aca="false">2*F3</f>
-        <v>0.8418</v>
-      </c>
-      <c r="G4" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="23" t="n">
-        <f aca="false">2*H3</f>
-        <v>1.2718</v>
-      </c>
-      <c r="I4" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="24" t="n">
-        <f aca="false">2*J3</f>
-        <v>5.1808</v>
-      </c>
-      <c r="K4" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="24" t="n">
-        <f aca="false">2*L3</f>
-        <v>5.8774</v>
-      </c>
-      <c r="M4" s="22" t="n">
-        <v>0</v>
+      <c r="B4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="E4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="H4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="K4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="27" t="n">
+        <v>1.00001</v>
+      </c>
+      <c r="N4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="27" t="n">
+        <v>1.00001</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +1978,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1961,223 +1986,523 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="16.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="7.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="7.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="7.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="7.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="7.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="7.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="7.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="7.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="25" width="7.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="25" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="25" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="O1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="26" t="s">
         <v>79</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B2" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="E2" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="F2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="H2" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="J2" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="K2" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="L2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="M2" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="N2" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="O2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="P2" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B3" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="E3" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="F3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="H3" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="J3" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="K3" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="L3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="M3" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="N3" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="O3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B4" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="E4" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="F4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="H4" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="J4" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="K4" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="L4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="M4" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
       </c>
       <c r="N4" s="27" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="O4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="27" t="n">
-        <v>1.00001</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" s="27" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2192,549 +2517,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:P10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="7.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="7.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="7.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="7.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="25" width="7.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="25" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="25" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.59"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="H2" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I2" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="K2" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L2" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="N2" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="O2" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="27" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C3" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="H3" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I3" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="K3" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L3" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="N3" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="O3" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="27" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="E4" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="H4" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="K4" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="27" t="n">
-        <v>100</v>
-      </c>
-      <c r="N4" s="27" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="O4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="27" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P8" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P9" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="P10" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2754,12 +2536,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="11.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="8.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="14.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="48.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2767,37 +2549,37 @@
         <v>33</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>90</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,7 +2587,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2825,7 +2607,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,13 +2615,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="D3" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>96</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2853,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2861,7 +2643,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -2881,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2914,11 +2696,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="2.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="5.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="5.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="3.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3089,7 +2871,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="25.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,7 +2951,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="18.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="4" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="4" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -3301,15 +3083,15 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="6.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,60 +3270,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3559,72 +3354,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="4.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>51</v>
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="15" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="C2" s="15" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="15" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="C3" s="15" t="n">
+        <v>-2.6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>52</v>
+      <c r="B4" s="15" t="n">
+        <v>-27.7</v>
+      </c>
+      <c r="C4" s="15" t="n">
+        <v>-27.7</v>
       </c>
     </row>
   </sheetData>
@@ -3643,62 +3428,131 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>55</v>
       </c>
+      <c r="C1" s="16" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="15" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="C2" s="15" t="n">
-        <v>3.2</v>
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="17" t="n">
+        <v>0.0001705</v>
+      </c>
+      <c r="C2" s="17" t="n">
+        <v>0.0001705</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="15" t="n">
-        <v>-2.6</v>
-      </c>
-      <c r="C3" s="15" t="n">
-        <v>-2.6</v>
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="17" t="n">
+        <v>1.4E-006</v>
+      </c>
+      <c r="C3" s="17" t="n">
+        <v>1.4E-006</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="15" t="n">
-        <v>-27.7</v>
-      </c>
-      <c r="C4" s="15" t="n">
-        <v>-27.7</v>
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="17" t="n">
+        <v>3.65E-006</v>
+      </c>
+      <c r="C4" s="17" t="n">
+        <v>3.65E-006</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="18" t="n">
+        <f aca="false">0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="18" t="n">
+        <f aca="false">0.01</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="18" t="n">
+        <f aca="false">0.0006</f>
+        <v>0.0006</v>
+      </c>
+      <c r="C6" s="18" t="n">
+        <f aca="false">0.0006</f>
+        <v>0.0006</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="18" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C7" s="18" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="18" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="18" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="C9" s="18" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="18" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C10" s="18" t="n">
+        <v>0.0001</v>
       </c>
     </row>
   </sheetData>
@@ -3717,131 +3571,198 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>40</v>
+    <row r="1" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="17" t="n">
-        <v>0.0001705</v>
-      </c>
-      <c r="C2" s="17" t="n">
-        <v>0.0001705</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="17" t="n">
-        <v>1.4E-006</v>
-      </c>
-      <c r="C3" s="17" t="n">
-        <v>1.4E-006</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="17" t="n">
-        <v>3.65E-006</v>
-      </c>
-      <c r="C4" s="17" t="n">
-        <v>3.65E-006</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="18" t="n">
-        <f aca="false">0.01</f>
-        <v>0.01</v>
-      </c>
-      <c r="C5" s="18" t="n">
-        <f aca="false">0.01</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="18" t="n">
-        <f aca="false">0.0006</f>
-        <v>0.0006</v>
-      </c>
-      <c r="C6" s="18" t="n">
-        <f aca="false">0.0006</f>
-        <v>0.0006</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="18" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="C7" s="18" t="n">
-        <v>0.0001</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="18" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="C8" s="18" t="n">
-        <v>0.0001</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="18" t="n">
-        <v>0.0015</v>
-      </c>
-      <c r="C9" s="18" t="n">
-        <v>0.0015</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="18" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="C10" s="18" t="n">
-        <v>0.0001</v>
+        <v>58</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="21" t="n">
+        <v>1.121</v>
+      </c>
+      <c r="C2" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="23" t="n">
+        <v>0.1601</v>
+      </c>
+      <c r="E2" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="23" t="n">
+        <v>0.4209</v>
+      </c>
+      <c r="G2" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="23" t="n">
+        <v>0.6359</v>
+      </c>
+      <c r="I2" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="24" t="n">
+        <v>2.5904</v>
+      </c>
+      <c r="K2" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="24" t="n">
+        <v>2.9387</v>
+      </c>
+      <c r="M2" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="21" t="n">
+        <v>1.121</v>
+      </c>
+      <c r="C3" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="23" t="n">
+        <v>0.1601</v>
+      </c>
+      <c r="E3" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="23" t="n">
+        <v>0.4209</v>
+      </c>
+      <c r="G3" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="23" t="n">
+        <v>0.6359</v>
+      </c>
+      <c r="I3" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="24" t="n">
+        <v>2.5904</v>
+      </c>
+      <c r="K3" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24" t="n">
+        <v>2.9387</v>
+      </c>
+      <c r="M3" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="20" customFormat="true" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="21" t="n">
+        <f aca="false">2*B3</f>
+        <v>2.242</v>
+      </c>
+      <c r="C4" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="23" t="n">
+        <f aca="false">2*D3</f>
+        <v>0.3202</v>
+      </c>
+      <c r="E4" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="23" t="n">
+        <f aca="false">2*F3</f>
+        <v>0.8418</v>
+      </c>
+      <c r="G4" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="23" t="n">
+        <f aca="false">2*H3</f>
+        <v>1.2718</v>
+      </c>
+      <c r="I4" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="24" t="n">
+        <f aca="false">2*J3</f>
+        <v>5.1808</v>
+      </c>
+      <c r="K4" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24" t="n">
+        <f aca="false">2*L3</f>
+        <v>5.8774</v>
+      </c>
+      <c r="M4" s="22" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>